<commit_message>
Journal de travail - François
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,10 +39,10 @@
     <t>Albert Einstein</t>
   </si>
   <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
+    <t xml:space="preserve">Choix de la proposition du projet </t>
+  </si>
+  <si>
+    <t>Lecture de la proposition</t>
   </si>
 </sst>
 </file>
@@ -446,26 +446,26 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>43150</v>
       </c>
@@ -484,10 +484,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="8">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>43152</v>
       </c>
@@ -495,141 +495,141 @@
         <v>7</v>
       </c>
       <c r="C6" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
journal de travail François Burgener
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD589CEF-907A-4009-8C72-8C749C5AD2EB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -36,23 +37,77 @@
     <t>Journal de travail</t>
   </si>
   <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choix de la proposition du projet </t>
-  </si>
-  <si>
-    <t>Lecture de la proposition</t>
+    <t>François Burgener</t>
+  </si>
+  <si>
+    <t>Discution du choix de l'architecture de notre application</t>
+  </si>
+  <si>
+    <t>Discussion sur la proposition du sujets</t>
+  </si>
+  <si>
+    <t>Lecture du sujet</t>
+  </si>
+  <si>
+    <t>Rédaction détaillé des fonctionnalités (Budget,catégorisation et choix de devises) et discution sur les necessité du projet</t>
+  </si>
+  <si>
+    <t>Elaboration du cahier des charges, discussion en groupe pour l'achèvement des fonctionnalités et le choix de l'architecture</t>
+  </si>
+  <si>
+    <t>Feedback et discution avec le professeur de notre sujet</t>
+  </si>
+  <si>
+    <t>Finalisation du planning et la distribution des heure. Relecture du cahier des charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elaboration des croquis des fenêtes des interface graphique  </t>
+  </si>
+  <si>
+    <t>Discution du cahier des charges avec le professeur</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Elaboration des croquis des fenêtes des interface graphique (vue global,Budget,vue budget,transaction) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Discution,correction sur les maquettes ainsi que notre schéma relationel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apprentissage javaFX. Visionnage de tutoriel sur youtube et quelque test </t>
+  </si>
+  <si>
+    <t>Apprentissage javaFX. J'ai lu le cours de openclassroom sur javaFX. J'ai regardé des vidéo et j'ai fait des petit test pour prendre en main  le code</t>
+  </si>
+  <si>
+    <t>Apprentissage javaFX, interface avec FXML au lieu du code. Début de la fenêtre de connexion et création d'un compte utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuer sur la fenêtre de connexion, pkus sur le design </t>
+  </si>
+  <si>
+    <t>Quelque correction a propos des containers utilisés dans la vue de login/register</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +141,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -439,11 +501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,10 +543,10 @@
         <v>43150</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,81 +554,165 @@
         <v>43152</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="8">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="3">
+        <v>43157</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
+      <c r="A8" s="3">
+        <v>43157</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>43158</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>43161</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>43163</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>43163</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>43164</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>43169</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>43170</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
+      <c r="A16" s="3">
+        <v>43171</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>43171</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>43176</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
+      <c r="A19" s="3">
+        <v>43177</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>43178</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -629,7 +775,7 @@
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>0.5</v>
+        <v>28.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj journal de travail francois burgener
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A465B2E-CB3D-4844-8BB8-3391884AD5B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -113,11 +114,41 @@
   <si>
     <t>Continuer sur la fenêtre qui liste des compte bancaire</t>
   </si>
+  <si>
+    <t>Création de la fenêtre de création d'un compte bancaire, Problème d'interaction avec la fenêtre principale. Je n'arrive pas a faire communiquer les deux controlleur (Controlleur_BankAccount et Controlleur_createBankAccount)</t>
+  </si>
+  <si>
+    <t>Résolution du problème javaFX et maven</t>
+  </si>
+  <si>
+    <t>Intégration du javaFX dans le projet maven, problème : il n'arrive pas a load les fichier fxml. Recherche du problème</t>
+  </si>
+  <si>
+    <t>création du ppt</t>
+  </si>
+  <si>
+    <t>présentation intermédiaire de notre projet</t>
+  </si>
+  <si>
+    <t>Ajout des fonction de la BLL dans le controlleur du loginRegister</t>
+  </si>
+  <si>
+    <t>création d'un compte utilisateur terminé</t>
+  </si>
+  <si>
+    <t>Mise au point de ce qu'il reste a faire sur l'interface graphique</t>
+  </si>
+  <si>
+    <t>Modification du rapport de la partie controlleur du compte bancaire</t>
+  </si>
+  <si>
+    <t>Ajout de l'évenement sur le compte bancaire</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -515,11 +546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,33 +834,208 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>43199</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="8"/>
+      <c r="A29" s="3">
+        <v>43203</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>43203</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="3">
+        <v>43205</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="3">
+        <v>43206</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>43206</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>43207</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>43213</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>43218</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>43218</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="8"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="8"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="9">
-        <f>SUM(C5:C31)</f>
-        <v>40</v>
+      <c r="C55" s="9">
+        <f>SUM(C5:C54)</f>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj journal de travail françois burgener
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A465B2E-CB3D-4844-8BB8-3391884AD5B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAD6AE0-5B64-4C8F-B179-20913DF958B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Ajout de l'évenement sur le compte bancaire</t>
+  </si>
+  <si>
+    <t>Transfère des données du compte bancaire du controlleur bankAccount au controlleur detailBankAccount. Quelque modification dans la fenêtre du détail d'un compte bancaire.  Modification des champs et test des graphiques</t>
+  </si>
+  <si>
+    <t>Rapport sur la partie détail compte bancaire</t>
   </si>
 </sst>
 </file>
@@ -549,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,15 +950,27 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="8"/>
+    <row r="38" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>43218</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="8"/>
+      <c r="A39" s="3">
+        <v>43218</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
@@ -1035,7 +1053,7 @@
       </c>
       <c r="C55" s="9">
         <f>SUM(C5:C54)</f>
-        <v>48</v>
+        <v>50.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maj jdd francois + modif code
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1B3FFE-57FB-4978-943A-48D79DBEF8D9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AF3734-548F-4213-AB23-72DAF7C5EEFF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,27 @@
   </si>
   <si>
     <t>Commencement du dashboard graphique/liste des transaction</t>
+  </si>
+  <si>
+    <t>11h30</t>
+  </si>
+  <si>
+    <t>Mise en forme des transaction dans le dahboard</t>
+  </si>
+  <si>
+    <t>12h45</t>
+  </si>
+  <si>
+    <t>Ajout du pieChart</t>
+  </si>
+  <si>
+    <t>13h15</t>
+  </si>
+  <si>
+    <t>Correction graphique dashboard</t>
+  </si>
+  <si>
+    <t>Problème général dans l'application. Recherche du problème si c'était du coté GUI</t>
   </si>
 </sst>
 </file>
@@ -382,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -430,6 +451,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1408,7 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>43227</v>
       </c>
@@ -1398,11 +1422,11 @@
         <v>11</v>
       </c>
       <c r="E49" s="16">
-        <f>SUM(C49:C58)</f>
-        <v>8.25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <f>SUM(C49:C62)</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>43227</v>
       </c>
@@ -1415,7 +1439,7 @@
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>43229</v>
       </c>
@@ -1428,7 +1452,7 @@
       <c r="D51" s="17"/>
       <c r="E51" s="17"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>43230</v>
       </c>
@@ -1441,7 +1465,7 @@
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>43230</v>
       </c>
@@ -1454,7 +1478,7 @@
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>43230</v>
       </c>
@@ -1467,7 +1491,7 @@
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>43230</v>
       </c>
@@ -1480,7 +1504,7 @@
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>43230</v>
       </c>
@@ -1493,7 +1517,7 @@
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>43230</v>
       </c>
@@ -1506,7 +1530,7 @@
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
     </row>
-    <row r="58" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>43230</v>
       </c>
@@ -1516,37 +1540,113 @@
       <c r="C58" s="10">
         <v>1.25</v>
       </c>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="8"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="8"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="8"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <v>43233</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="9">
-        <f>SUM(C5:C61)</f>
-        <v>80</v>
+      <c r="C67" s="9">
+        <f>SUM(C5:C66)</f>
+        <v>83.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D49:D58"/>
-    <mergeCell ref="E49:E58"/>
+    <mergeCell ref="D49:D62"/>
+    <mergeCell ref="E49:E62"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D41"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D19"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="E13:E15"/>
@@ -1561,13 +1661,6 @@
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D41"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
pieChart + maj jdt francois
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB468A66-58AF-4B6D-90D2-0A6637C81180}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -240,11 +239,23 @@
   <si>
     <t>Modification d'un budget</t>
   </si>
+  <si>
+    <t>Ajout des images à tout les bouton (add/supp/retour/edit/setting)</t>
+  </si>
+  <si>
+    <t>Calcule des dépense sur plusieurs catégorie</t>
+  </si>
+  <si>
+    <t>Progresse bar sur les budget</t>
+  </si>
+  <si>
+    <t>Graphique en camembert budget</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -446,6 +457,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -457,15 +477,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,11 +757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,10 +779,10 @@
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="23"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -803,10 +814,10 @@
       <c r="C5" s="10">
         <v>0.5</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="20">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="20">
         <f>SUM(C5:C6)</f>
         <v>0.75</v>
       </c>
@@ -821,8 +832,8 @@
       <c r="C6" s="10">
         <v>0.25</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -834,10 +845,10 @@
       <c r="C7" s="10">
         <v>0.5</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="20">
         <v>2</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="20">
         <f>SUM(C7:C12)</f>
         <v>13</v>
       </c>
@@ -852,8 +863,8 @@
       <c r="C8" s="10">
         <v>1</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -865,8 +876,8 @@
       <c r="C9" s="10">
         <v>2</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -878,8 +889,8 @@
       <c r="C10" s="10">
         <v>3</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -891,8 +902,8 @@
       <c r="C11" s="10">
         <v>4.5</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -904,8 +915,8 @@
       <c r="C12" s="10">
         <v>2</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -917,10 +928,10 @@
       <c r="C13" s="10">
         <v>1.5</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="20">
         <v>3</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="20">
         <f>SUM(C13:C15)</f>
         <v>6</v>
       </c>
@@ -935,8 +946,8 @@
       <c r="C14" s="10">
         <v>2.5</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -948,8 +959,8 @@
       <c r="C15" s="10">
         <v>2</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -961,10 +972,10 @@
       <c r="C16" s="10">
         <v>0.5</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="20">
         <v>4</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="20">
         <f>SUM(C16:C19)</f>
         <v>8</v>
       </c>
@@ -979,8 +990,8 @@
       <c r="C17" s="10">
         <v>1</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -992,8 +1003,8 @@
       <c r="C18" s="10">
         <v>5</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
@@ -1005,8 +1016,8 @@
       <c r="C19" s="10">
         <v>1.5</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1018,10 +1029,10 @@
       <c r="C20" s="10">
         <v>0.5</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="20">
         <v>5</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="20">
         <f>SUM(C20:C23)</f>
         <v>6.5</v>
       </c>
@@ -1036,8 +1047,8 @@
       <c r="C21" s="10">
         <v>1.5</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1049,8 +1060,8 @@
       <c r="C22" s="10">
         <v>2</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -1062,8 +1073,8 @@
       <c r="C23" s="10">
         <v>2.5</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1075,10 +1086,10 @@
       <c r="C24" s="10">
         <v>1.5</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="20">
         <v>6</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="20">
         <f>SUM(C24:C26)</f>
         <v>3.75</v>
       </c>
@@ -1093,8 +1104,8 @@
       <c r="C25" s="10">
         <v>0.75</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
@@ -1106,8 +1117,8 @@
       <c r="C26" s="10">
         <v>1.5</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
@@ -1137,10 +1148,10 @@
       <c r="C28" s="10">
         <v>1</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="20">
         <v>7</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="20">
         <f>SUM(C28:C31)</f>
         <v>4.5</v>
       </c>
@@ -1155,8 +1166,8 @@
       <c r="C29" s="10">
         <v>1.5</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -1168,8 +1179,8 @@
       <c r="C30" s="10">
         <v>1.5</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
@@ -1181,8 +1192,8 @@
       <c r="C31" s="10">
         <v>0.5</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1194,10 +1205,10 @@
       <c r="C32" s="10">
         <v>0.25</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="20">
         <v>8</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="20">
         <f>SUM(C32:C34)</f>
         <v>1.25</v>
       </c>
@@ -1212,8 +1223,8 @@
       <c r="C33" s="10">
         <v>0.75</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -1225,8 +1236,8 @@
       <c r="C34" s="10">
         <v>0.25</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1238,10 +1249,10 @@
       <c r="C35" s="10">
         <v>1.5</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="20">
         <v>9</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="20">
         <f>SUM(C35:C41)</f>
         <v>8</v>
       </c>
@@ -1256,8 +1267,8 @@
       <c r="C36" s="10">
         <v>0.25</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
@@ -1269,8 +1280,8 @@
       <c r="C37" s="10">
         <v>0.5</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -1282,8 +1293,8 @@
       <c r="C38" s="10">
         <v>2</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -1295,8 +1306,8 @@
       <c r="C39" s="10">
         <v>0.5</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
@@ -1308,8 +1319,8 @@
       <c r="C40" s="10">
         <v>0.25</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
     </row>
     <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
@@ -1321,8 +1332,8 @@
       <c r="C41" s="10">
         <v>3</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -1334,10 +1345,10 @@
       <c r="C42" s="10">
         <v>2</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="20">
         <v>10</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="20">
         <f>SUM(C42:C48)</f>
         <v>18</v>
       </c>
@@ -1352,8 +1363,8 @@
       <c r="C43" s="10">
         <v>5</v>
       </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
@@ -1365,8 +1376,8 @@
       <c r="C44" s="10">
         <v>2</v>
       </c>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
@@ -1378,8 +1389,8 @@
       <c r="C45" s="15">
         <v>2.5</v>
       </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -1391,8 +1402,8 @@
       <c r="C46" s="10">
         <v>4</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -1404,8 +1415,8 @@
       <c r="C47" s="15">
         <v>0.75</v>
       </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
@@ -1417,8 +1428,8 @@
       <c r="C48" s="15">
         <v>1.75</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
@@ -1430,10 +1441,10 @@
       <c r="C49" s="10">
         <v>1.5</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="17">
         <v>11</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="20">
         <f>SUM(C49:C66)</f>
         <v>15</v>
       </c>
@@ -1448,8 +1459,8 @@
       <c r="C50" s="10">
         <v>0.25</v>
       </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="21"/>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
@@ -1461,8 +1472,8 @@
       <c r="C51" s="10">
         <v>1</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="21"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
@@ -1474,8 +1485,8 @@
       <c r="C52" s="10">
         <v>1</v>
       </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="21"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -1487,8 +1498,8 @@
       <c r="C53" s="10">
         <v>0.75</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="21"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
@@ -1500,8 +1511,8 @@
       <c r="C54" s="10">
         <v>0.75</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -1513,8 +1524,8 @@
       <c r="C55" s="10">
         <v>0.75</v>
       </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="21"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
@@ -1526,8 +1537,8 @@
       <c r="C56" s="10">
         <v>0.25</v>
       </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="21"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
@@ -1539,8 +1550,8 @@
       <c r="C57" s="10">
         <v>0.75</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="21"/>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
@@ -1552,8 +1563,8 @@
       <c r="C58" s="10">
         <v>1.25</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="21"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
@@ -1565,8 +1576,8 @@
       <c r="C59" s="10">
         <v>0.75</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="21"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
@@ -1578,8 +1589,8 @@
       <c r="C60" s="16">
         <v>0.5</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="21"/>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
@@ -1591,8 +1602,8 @@
       <c r="C61" s="10">
         <v>1.5</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="21"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
@@ -1604,8 +1615,8 @@
       <c r="C62" s="10">
         <v>0.5</v>
       </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="21"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
@@ -1617,8 +1628,8 @@
       <c r="C63" s="10">
         <v>0.5</v>
       </c>
-      <c r="D63" s="22"/>
-      <c r="E63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="21"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
@@ -1630,8 +1641,8 @@
       <c r="C64" s="15">
         <v>1</v>
       </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="21"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
@@ -1643,8 +1654,8 @@
       <c r="C65" s="10">
         <v>1</v>
       </c>
-      <c r="D65" s="22"/>
-      <c r="E65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="21"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
@@ -1656,28 +1667,65 @@
       <c r="C66" s="10">
         <v>1</v>
       </c>
-      <c r="D66" s="23"/>
-      <c r="E66" s="19"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="8"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="22"/>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>43204</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D67" s="20">
+        <v>12</v>
+      </c>
+      <c r="E67" s="20">
+        <f>SUM(C67:C70)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="8"/>
+      <c r="A68" s="3">
+        <v>43204</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="8"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="8"/>
+      <c r="A69" s="3">
+        <v>43204</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>43234</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
@@ -1700,27 +1748,13 @@
       </c>
       <c r="C74" s="9">
         <f>SUM(C5:C73)</f>
-        <v>86.75</v>
+        <v>89.75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="D49:D66"/>
-    <mergeCell ref="E49:E66"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E41"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D41"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D19"/>
+  <mergeCells count="25">
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="E67:E70"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="E13:E15"/>
@@ -1728,6 +1762,22 @@
     <mergeCell ref="D42:D48"/>
     <mergeCell ref="E42:E48"/>
     <mergeCell ref="E20:E23"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D41"/>
+    <mergeCell ref="D49:D66"/>
+    <mergeCell ref="E49:E66"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="E35:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
budget et jdt francois
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Graphique en camembert budget</t>
+  </si>
+  <si>
+    <t>Quelque modif dans les budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peaufinage du code </t>
   </si>
 </sst>
 </file>
@@ -457,15 +463,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -477,6 +474,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+      <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,10 +785,10 @@
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -814,10 +820,10 @@
       <c r="C5" s="10">
         <v>0.5</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <v>1</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="17">
         <f>SUM(C5:C6)</f>
         <v>0.75</v>
       </c>
@@ -832,8 +838,8 @@
       <c r="C6" s="10">
         <v>0.25</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -845,10 +851,10 @@
       <c r="C7" s="10">
         <v>0.5</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <v>2</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <f>SUM(C7:C12)</f>
         <v>13</v>
       </c>
@@ -863,8 +869,8 @@
       <c r="C8" s="10">
         <v>1</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -876,8 +882,8 @@
       <c r="C9" s="10">
         <v>2</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -889,8 +895,8 @@
       <c r="C10" s="10">
         <v>3</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -902,8 +908,8 @@
       <c r="C11" s="10">
         <v>4.5</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -915,8 +921,8 @@
       <c r="C12" s="10">
         <v>2</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -928,10 +934,10 @@
       <c r="C13" s="10">
         <v>1.5</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="17">
         <v>3</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="17">
         <f>SUM(C13:C15)</f>
         <v>6</v>
       </c>
@@ -946,8 +952,8 @@
       <c r="C14" s="10">
         <v>2.5</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -959,8 +965,8 @@
       <c r="C15" s="10">
         <v>2</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -972,10 +978,10 @@
       <c r="C16" s="10">
         <v>0.5</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="17">
         <v>4</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="17">
         <f>SUM(C16:C19)</f>
         <v>8</v>
       </c>
@@ -990,8 +996,8 @@
       <c r="C17" s="10">
         <v>1</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1003,8 +1009,8 @@
       <c r="C18" s="10">
         <v>5</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
@@ -1016,8 +1022,8 @@
       <c r="C19" s="10">
         <v>1.5</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1029,10 +1035,10 @@
       <c r="C20" s="10">
         <v>0.5</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="17">
         <v>5</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="17">
         <f>SUM(C20:C23)</f>
         <v>6.5</v>
       </c>
@@ -1047,8 +1053,8 @@
       <c r="C21" s="10">
         <v>1.5</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1060,8 +1066,8 @@
       <c r="C22" s="10">
         <v>2</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -1073,8 +1079,8 @@
       <c r="C23" s="10">
         <v>2.5</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1086,10 +1092,10 @@
       <c r="C24" s="10">
         <v>1.5</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="17">
         <v>6</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="17">
         <f>SUM(C24:C26)</f>
         <v>3.75</v>
       </c>
@@ -1104,8 +1110,8 @@
       <c r="C25" s="10">
         <v>0.75</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
@@ -1117,8 +1123,8 @@
       <c r="C26" s="10">
         <v>1.5</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
@@ -1148,10 +1154,10 @@
       <c r="C28" s="10">
         <v>1</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="17">
         <v>7</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="17">
         <f>SUM(C28:C31)</f>
         <v>4.5</v>
       </c>
@@ -1166,8 +1172,8 @@
       <c r="C29" s="10">
         <v>1.5</v>
       </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -1179,8 +1185,8 @@
       <c r="C30" s="10">
         <v>1.5</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
@@ -1192,8 +1198,8 @@
       <c r="C31" s="10">
         <v>0.5</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1205,10 +1211,10 @@
       <c r="C32" s="10">
         <v>0.25</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="17">
         <v>8</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="17">
         <f>SUM(C32:C34)</f>
         <v>1.25</v>
       </c>
@@ -1223,8 +1229,8 @@
       <c r="C33" s="10">
         <v>0.75</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -1236,8 +1242,8 @@
       <c r="C34" s="10">
         <v>0.25</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1249,10 +1255,10 @@
       <c r="C35" s="10">
         <v>1.5</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="17">
         <v>9</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="17">
         <f>SUM(C35:C41)</f>
         <v>8</v>
       </c>
@@ -1267,8 +1273,8 @@
       <c r="C36" s="10">
         <v>0.25</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
@@ -1280,8 +1286,8 @@
       <c r="C37" s="10">
         <v>0.5</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -1293,8 +1299,8 @@
       <c r="C38" s="10">
         <v>2</v>
       </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -1306,8 +1312,8 @@
       <c r="C39" s="10">
         <v>0.5</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
@@ -1319,8 +1325,8 @@
       <c r="C40" s="10">
         <v>0.25</v>
       </c>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
@@ -1332,8 +1338,8 @@
       <c r="C41" s="10">
         <v>3</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -1345,10 +1351,10 @@
       <c r="C42" s="10">
         <v>2</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="17">
         <v>10</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="17">
         <f>SUM(C42:C48)</f>
         <v>18</v>
       </c>
@@ -1363,8 +1369,8 @@
       <c r="C43" s="10">
         <v>5</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
@@ -1376,8 +1382,8 @@
       <c r="C44" s="10">
         <v>2</v>
       </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
@@ -1389,8 +1395,8 @@
       <c r="C45" s="15">
         <v>2.5</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -1402,8 +1408,8 @@
       <c r="C46" s="10">
         <v>4</v>
       </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -1415,8 +1421,8 @@
       <c r="C47" s="15">
         <v>0.75</v>
       </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
@@ -1428,8 +1434,8 @@
       <c r="C48" s="15">
         <v>1.75</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
@@ -1441,10 +1447,10 @@
       <c r="C49" s="10">
         <v>1.5</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="21">
         <v>11</v>
       </c>
-      <c r="E49" s="20">
+      <c r="E49" s="17">
         <f>SUM(C49:C66)</f>
         <v>15</v>
       </c>
@@ -1459,8 +1465,8 @@
       <c r="C50" s="10">
         <v>0.25</v>
       </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="21"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
@@ -1472,8 +1478,8 @@
       <c r="C51" s="10">
         <v>1</v>
       </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="21"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
@@ -1485,8 +1491,8 @@
       <c r="C52" s="10">
         <v>1</v>
       </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="21"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="18"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -1498,8 +1504,8 @@
       <c r="C53" s="10">
         <v>0.75</v>
       </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="21"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="18"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
@@ -1511,8 +1517,8 @@
       <c r="C54" s="10">
         <v>0.75</v>
       </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="21"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="18"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -1524,8 +1530,8 @@
       <c r="C55" s="10">
         <v>0.75</v>
       </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="21"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="18"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
@@ -1537,8 +1543,8 @@
       <c r="C56" s="10">
         <v>0.25</v>
       </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="21"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
@@ -1550,8 +1556,8 @@
       <c r="C57" s="10">
         <v>0.75</v>
       </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="21"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="18"/>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
@@ -1563,8 +1569,8 @@
       <c r="C58" s="10">
         <v>1.25</v>
       </c>
-      <c r="D58" s="18"/>
-      <c r="E58" s="21"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
@@ -1576,8 +1582,8 @@
       <c r="C59" s="10">
         <v>0.75</v>
       </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="21"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="18"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
@@ -1589,8 +1595,8 @@
       <c r="C60" s="16">
         <v>0.5</v>
       </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="21"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="18"/>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
@@ -1602,8 +1608,8 @@
       <c r="C61" s="10">
         <v>1.5</v>
       </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="21"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="18"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
@@ -1615,8 +1621,8 @@
       <c r="C62" s="10">
         <v>0.5</v>
       </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="21"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="18"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
@@ -1628,8 +1634,8 @@
       <c r="C63" s="10">
         <v>0.5</v>
       </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="21"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="18"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
@@ -1641,8 +1647,8 @@
       <c r="C64" s="15">
         <v>1</v>
       </c>
-      <c r="D64" s="18"/>
-      <c r="E64" s="21"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="18"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
@@ -1654,8 +1660,8 @@
       <c r="C65" s="10">
         <v>1</v>
       </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="21"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="18"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
@@ -1667,8 +1673,8 @@
       <c r="C66" s="10">
         <v>1</v>
       </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="22"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="19"/>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
@@ -1680,12 +1686,12 @@
       <c r="C67" s="10">
         <v>0.75</v>
       </c>
-      <c r="D67" s="20">
+      <c r="D67" s="17">
         <v>12</v>
       </c>
-      <c r="E67" s="20">
-        <f>SUM(C67:C70)</f>
-        <v>3</v>
+      <c r="E67" s="17">
+        <f>SUM(C67:C73)</f>
+        <v>6.75</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,8 +1704,8 @@
       <c r="C68" s="10">
         <v>0.75</v>
       </c>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
@@ -1711,10 +1717,10 @@
       <c r="C69" s="10">
         <v>0.75</v>
       </c>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>43234</v>
       </c>
@@ -1724,37 +1730,69 @@
       <c r="C70" s="10">
         <v>0.75</v>
       </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="8"/>
+      <c r="A71" s="3">
+        <v>43234</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="8"/>
+      <c r="A72" s="3">
+        <v>43235</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
+        <v>43236</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="5" t="s">
+      <c r="A74" s="3"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="9">
-        <f>SUM(C5:C73)</f>
-        <v>89.75</v>
+      <c r="C76" s="9">
+        <f>SUM(C5:C75)</f>
+        <v>93.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="E67:E70"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="E13:E15"/>
@@ -1762,22 +1800,24 @@
     <mergeCell ref="D42:D48"/>
     <mergeCell ref="E42:E48"/>
     <mergeCell ref="E20:E23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D41"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D41"/>
-    <mergeCell ref="D49:D66"/>
-    <mergeCell ref="E49:E66"/>
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="E32:E34"/>
     <mergeCell ref="E35:E41"/>
+    <mergeCell ref="D49:D66"/>
+    <mergeCell ref="E49:E66"/>
+    <mergeCell ref="D67:D73"/>
+    <mergeCell ref="E67:E73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rapport et jdt francois
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273FABFF-7CB8-4116-836D-8B2C7D64480B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -269,11 +270,17 @@
   <si>
     <t xml:space="preserve">rapport sur la partie transaction </t>
   </si>
+  <si>
+    <t>Continuer sur le rapport transaction, et commencement de la partie budget</t>
+  </si>
+  <si>
+    <t>Continuation des rapports (budget et dashboard)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -435,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -475,18 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,8 +491,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -778,11 +782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="79" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,10 +804,10 @@
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="23"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -835,10 +839,10 @@
       <c r="C5" s="10">
         <v>0.5</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="20">
         <v>1</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="20">
         <f>SUM(C5:C6)</f>
         <v>0.75</v>
       </c>
@@ -853,8 +857,8 @@
       <c r="C6" s="10">
         <v>0.25</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -866,10 +870,10 @@
       <c r="C7" s="10">
         <v>0.5</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="20">
         <v>2</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="20">
         <f>SUM(C7:C12)</f>
         <v>13</v>
       </c>
@@ -884,8 +888,8 @@
       <c r="C8" s="10">
         <v>1</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -897,8 +901,8 @@
       <c r="C9" s="10">
         <v>2</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -910,8 +914,8 @@
       <c r="C10" s="10">
         <v>3</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -923,8 +927,8 @@
       <c r="C11" s="10">
         <v>4.5</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -936,8 +940,8 @@
       <c r="C12" s="10">
         <v>2</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -949,10 +953,10 @@
       <c r="C13" s="10">
         <v>1.5</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="20">
         <v>3</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="20">
         <f>SUM(C13:C15)</f>
         <v>6</v>
       </c>
@@ -967,8 +971,8 @@
       <c r="C14" s="10">
         <v>2.5</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -980,8 +984,8 @@
       <c r="C15" s="10">
         <v>2</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -993,10 +997,10 @@
       <c r="C16" s="10">
         <v>0.5</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="20">
         <v>4</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="20">
         <f>SUM(C16:C19)</f>
         <v>8</v>
       </c>
@@ -1011,8 +1015,8 @@
       <c r="C17" s="10">
         <v>1</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1024,8 +1028,8 @@
       <c r="C18" s="10">
         <v>5</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
@@ -1037,8 +1041,8 @@
       <c r="C19" s="10">
         <v>1.5</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1050,10 +1054,10 @@
       <c r="C20" s="10">
         <v>0.5</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="20">
         <v>5</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="20">
         <f>SUM(C20:C23)</f>
         <v>6.5</v>
       </c>
@@ -1068,8 +1072,8 @@
       <c r="C21" s="10">
         <v>1.5</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1081,8 +1085,8 @@
       <c r="C22" s="10">
         <v>2</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -1094,8 +1098,8 @@
       <c r="C23" s="10">
         <v>2.5</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1107,10 +1111,10 @@
       <c r="C24" s="10">
         <v>1.5</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="20">
         <v>6</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="20">
         <f>SUM(C24:C26)</f>
         <v>3.75</v>
       </c>
@@ -1125,8 +1129,8 @@
       <c r="C25" s="10">
         <v>0.75</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
@@ -1138,8 +1142,8 @@
       <c r="C26" s="10">
         <v>1.5</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
@@ -1169,10 +1173,10 @@
       <c r="C28" s="10">
         <v>1</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="20">
         <v>7</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="20">
         <f>SUM(C28:C31)</f>
         <v>4.5</v>
       </c>
@@ -1187,8 +1191,8 @@
       <c r="C29" s="10">
         <v>1.5</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -1200,8 +1204,8 @@
       <c r="C30" s="10">
         <v>1.5</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
@@ -1213,8 +1217,8 @@
       <c r="C31" s="10">
         <v>0.5</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1226,10 +1230,10 @@
       <c r="C32" s="10">
         <v>0.25</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="20">
         <v>8</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="20">
         <f>SUM(C32:C34)</f>
         <v>1.25</v>
       </c>
@@ -1244,8 +1248,8 @@
       <c r="C33" s="10">
         <v>0.75</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
@@ -1257,8 +1261,8 @@
       <c r="C34" s="10">
         <v>0.25</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1270,10 +1274,10 @@
       <c r="C35" s="10">
         <v>1.5</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="20">
         <v>9</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="20">
         <f>SUM(C35:C41)</f>
         <v>8</v>
       </c>
@@ -1288,8 +1292,8 @@
       <c r="C36" s="10">
         <v>0.25</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
@@ -1301,8 +1305,8 @@
       <c r="C37" s="10">
         <v>0.5</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -1314,8 +1318,8 @@
       <c r="C38" s="10">
         <v>2</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -1327,8 +1331,8 @@
       <c r="C39" s="10">
         <v>0.5</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
@@ -1340,8 +1344,8 @@
       <c r="C40" s="10">
         <v>0.25</v>
       </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
     </row>
     <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
@@ -1353,8 +1357,8 @@
       <c r="C41" s="10">
         <v>3</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -1366,10 +1370,10 @@
       <c r="C42" s="10">
         <v>2</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="20">
         <v>10</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="20">
         <f>SUM(C42:C48)</f>
         <v>18</v>
       </c>
@@ -1384,8 +1388,8 @@
       <c r="C43" s="10">
         <v>5</v>
       </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
@@ -1397,8 +1401,8 @@
       <c r="C44" s="10">
         <v>2</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
@@ -1410,8 +1414,8 @@
       <c r="C45" s="15">
         <v>2.5</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -1423,8 +1427,8 @@
       <c r="C46" s="10">
         <v>4</v>
       </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -1436,8 +1440,8 @@
       <c r="C47" s="15">
         <v>0.75</v>
       </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
@@ -1449,8 +1453,8 @@
       <c r="C48" s="15">
         <v>1.75</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
@@ -1462,10 +1466,10 @@
       <c r="C49" s="10">
         <v>1.5</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="17">
         <v>11</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="20">
         <f>SUM(C49:C66)</f>
         <v>15</v>
       </c>
@@ -1480,8 +1484,8 @@
       <c r="C50" s="10">
         <v>0.25</v>
       </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="19"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="21"/>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
@@ -1493,8 +1497,8 @@
       <c r="C51" s="10">
         <v>1</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="19"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="21"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
@@ -1506,8 +1510,8 @@
       <c r="C52" s="10">
         <v>1</v>
       </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="19"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="21"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -1519,8 +1523,8 @@
       <c r="C53" s="10">
         <v>0.75</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="19"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="21"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
@@ -1532,8 +1536,8 @@
       <c r="C54" s="10">
         <v>0.75</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="19"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -1545,8 +1549,8 @@
       <c r="C55" s="10">
         <v>0.75</v>
       </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="19"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="21"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
@@ -1558,8 +1562,8 @@
       <c r="C56" s="10">
         <v>0.25</v>
       </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="19"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="21"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
@@ -1571,8 +1575,8 @@
       <c r="C57" s="10">
         <v>0.75</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="19"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="21"/>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
@@ -1584,8 +1588,8 @@
       <c r="C58" s="10">
         <v>1.25</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="19"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="21"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
@@ -1597,8 +1601,8 @@
       <c r="C59" s="10">
         <v>0.75</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="19"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="21"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
@@ -1610,8 +1614,8 @@
       <c r="C60" s="16">
         <v>0.5</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="19"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="21"/>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
@@ -1623,8 +1627,8 @@
       <c r="C61" s="10">
         <v>1.5</v>
       </c>
-      <c r="D61" s="22"/>
-      <c r="E61" s="19"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="21"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
@@ -1636,8 +1640,8 @@
       <c r="C62" s="10">
         <v>0.5</v>
       </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="19"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="21"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
@@ -1649,8 +1653,8 @@
       <c r="C63" s="10">
         <v>0.5</v>
       </c>
-      <c r="D63" s="22"/>
-      <c r="E63" s="19"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="21"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
@@ -1662,10 +1666,10 @@
       <c r="C64" s="15">
         <v>1</v>
       </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="19"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="18"/>
+      <c r="E64" s="21"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43233</v>
       </c>
@@ -1675,10 +1679,10 @@
       <c r="C65" s="10">
         <v>1</v>
       </c>
-      <c r="D65" s="22"/>
-      <c r="E65" s="19"/>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="18"/>
+      <c r="E65" s="21"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>43233</v>
       </c>
@@ -1688,10 +1692,10 @@
       <c r="C66" s="10">
         <v>1</v>
       </c>
-      <c r="D66" s="23"/>
-      <c r="E66" s="18"/>
-    </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D66" s="19"/>
+      <c r="E66" s="22"/>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>43204</v>
       </c>
@@ -1701,15 +1705,15 @@
       <c r="C67" s="10">
         <v>0.75</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D67" s="20">
         <v>12</v>
       </c>
-      <c r="E67" s="17">
-        <f>SUM(C67:C74)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="20">
+        <f>SUM(C67:C79)</f>
+        <v>16.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>43204</v>
       </c>
@@ -1719,10 +1723,10 @@
       <c r="C68" s="10">
         <v>0.75</v>
       </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>43204</v>
       </c>
@@ -1732,10 +1736,10 @@
       <c r="C69" s="10">
         <v>0.75</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>43234</v>
       </c>
@@ -1745,10 +1749,10 @@
       <c r="C70" s="10">
         <v>0.75</v>
       </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>43234</v>
       </c>
@@ -1758,10 +1762,10 @@
       <c r="C71" s="10">
         <v>0.5</v>
       </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>43235</v>
       </c>
@@ -1771,10 +1775,10 @@
       <c r="C72" s="10">
         <v>0.75</v>
       </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>43236</v>
       </c>
@@ -1784,10 +1788,10 @@
       <c r="C73" s="10">
         <v>2.5</v>
       </c>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>43236</v>
       </c>
@@ -1797,10 +1801,10 @@
       <c r="C74" s="10">
         <v>2.25</v>
       </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-    </row>
-    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>43236</v>
       </c>
@@ -1810,10 +1814,10 @@
       <c r="C75" s="10">
         <v>0.5</v>
       </c>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-    </row>
-    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+    </row>
+    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>43236</v>
       </c>
@@ -1823,10 +1827,10 @@
       <c r="C76" s="10">
         <v>3</v>
       </c>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>43237</v>
       </c>
@@ -1836,32 +1840,64 @@
       <c r="C77" s="10">
         <v>0.75</v>
       </c>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77">
-        <v>17.05</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="8"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="5" t="s">
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>43237</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <v>43237</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" s="10">
+        <v>2</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C79" s="9">
-        <f>SUM(C5:C78)</f>
-        <v>100</v>
+      <c r="C81" s="9">
+        <f>SUM(C5:C80)</f>
+        <v>103.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="E35:E41"/>
+    <mergeCell ref="D67:D79"/>
+    <mergeCell ref="E67:E79"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D41"/>
     <mergeCell ref="D49:D66"/>
     <mergeCell ref="E49:E66"/>
-    <mergeCell ref="D67:D74"/>
-    <mergeCell ref="E67:E74"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D12"/>
@@ -1874,15 +1910,6 @@
     <mergeCell ref="D42:D48"/>
     <mergeCell ref="E42:E48"/>
     <mergeCell ref="E20:E23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D41"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
jdt francois et resumé semaine ( à terminé)
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Francois.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273FABFF-7CB8-4116-836D-8B2C7D64480B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -276,11 +275,23 @@
   <si>
     <t>Continuation des rapports (budget et dashboard)</t>
   </si>
+  <si>
+    <t>Continuation sur le manuel d'utilisation</t>
+  </si>
+  <si>
+    <t>Finalisation du manuel d'utilisation</t>
+  </si>
+  <si>
+    <t>Bilan personnel</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport sur la partie compte bancaire</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -455,9 +466,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +489,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,26 +793,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="79" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="79" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
@@ -822,10 +833,10 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>45</v>
       </c>
     </row>
@@ -836,7 +847,7 @@
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>0.5</v>
       </c>
       <c r="D5" s="20">
@@ -854,7 +865,7 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>0.25</v>
       </c>
       <c r="D6" s="22"/>
@@ -867,7 +878,7 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>0.5</v>
       </c>
       <c r="D7" s="20">
@@ -885,20 +896,20 @@
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>43158</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>2</v>
       </c>
       <c r="D9" s="21"/>
@@ -911,33 +922,33 @@
       <c r="B10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>3</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>43163</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>4.5</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>43163</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>2</v>
       </c>
       <c r="D12" s="22"/>
@@ -950,7 +961,7 @@
       <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>1.5</v>
       </c>
       <c r="D13" s="20">
@@ -968,7 +979,7 @@
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>2.5</v>
       </c>
       <c r="D14" s="21"/>
@@ -981,7 +992,7 @@
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>2</v>
       </c>
       <c r="D15" s="22"/>
@@ -994,7 +1005,7 @@
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>0.5</v>
       </c>
       <c r="D16" s="20">
@@ -1012,20 +1023,20 @@
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>43176</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>5</v>
       </c>
       <c r="D18" s="21"/>
@@ -1038,7 +1049,7 @@
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>1.5</v>
       </c>
       <c r="D19" s="22"/>
@@ -1051,7 +1062,7 @@
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>0.5</v>
       </c>
       <c r="D20" s="20">
@@ -1069,7 +1080,7 @@
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>1.5</v>
       </c>
       <c r="D21" s="21"/>
@@ -1082,7 +1093,7 @@
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>2</v>
       </c>
       <c r="D22" s="21"/>
@@ -1095,7 +1106,7 @@
       <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <v>2.5</v>
       </c>
       <c r="D23" s="22"/>
@@ -1108,7 +1119,7 @@
       <c r="B24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>1.5</v>
       </c>
       <c r="D24" s="20">
@@ -1126,7 +1137,7 @@
       <c r="B25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>0.75</v>
       </c>
       <c r="D25" s="21"/>
@@ -1139,7 +1150,7 @@
       <c r="B26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>1.5</v>
       </c>
       <c r="D26" s="22"/>
@@ -1150,27 +1161,27 @@
         <v>43194</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="10">
+        <v>84</v>
+      </c>
+      <c r="C27" s="9">
         <v>2</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="13">
         <f>SUM(C27)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>43199</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <v>1</v>
       </c>
       <c r="D28" s="20">
@@ -1188,20 +1199,20 @@
       <c r="B29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>1.5</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>43203</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>1.5</v>
       </c>
       <c r="D30" s="21"/>
@@ -1214,7 +1225,7 @@
       <c r="B31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <v>0.5</v>
       </c>
       <c r="D31" s="22"/>
@@ -1227,7 +1238,7 @@
       <c r="B32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <v>0.25</v>
       </c>
       <c r="D32" s="20">
@@ -1238,14 +1249,14 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>43206</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>0.75</v>
       </c>
       <c r="D33" s="21"/>
@@ -1258,7 +1269,7 @@
       <c r="B34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <v>0.25</v>
       </c>
       <c r="D34" s="22"/>
@@ -1271,7 +1282,7 @@
       <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <v>1.5</v>
       </c>
       <c r="D35" s="20">
@@ -1289,7 +1300,7 @@
       <c r="B36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>0.25</v>
       </c>
       <c r="D36" s="21"/>
@@ -1302,20 +1313,20 @@
       <c r="B37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <v>0.5</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>43218</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>2</v>
       </c>
       <c r="D38" s="21"/>
@@ -1328,7 +1339,7 @@
       <c r="B39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="9">
         <v>0.5</v>
       </c>
       <c r="D39" s="21"/>
@@ -1341,7 +1352,7 @@
       <c r="B40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="9">
         <v>0.25</v>
       </c>
       <c r="D40" s="21"/>
@@ -1354,7 +1365,7 @@
       <c r="B41" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="9">
         <v>3</v>
       </c>
       <c r="D41" s="22"/>
@@ -1367,7 +1378,7 @@
       <c r="B42" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="9">
         <v>2</v>
       </c>
       <c r="D42" s="20">
@@ -1385,7 +1396,7 @@
       <c r="B43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="9">
         <v>5</v>
       </c>
       <c r="D43" s="21"/>
@@ -1398,7 +1409,7 @@
       <c r="B44" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="9">
         <v>2</v>
       </c>
       <c r="D44" s="21"/>
@@ -1411,7 +1422,7 @@
       <c r="B45" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="15">
+      <c r="C45" s="14">
         <v>2.5</v>
       </c>
       <c r="D45" s="21"/>
@@ -1424,7 +1435,7 @@
       <c r="B46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="9">
         <v>4</v>
       </c>
       <c r="D46" s="21"/>
@@ -1437,7 +1448,7 @@
       <c r="B47" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="14">
         <v>0.75</v>
       </c>
       <c r="D47" s="21"/>
@@ -1450,20 +1461,20 @@
       <c r="B48" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="14">
         <v>1.75</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>43227</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="9">
         <v>1.5</v>
       </c>
       <c r="D49" s="17">
@@ -1474,14 +1485,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>43227</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="9">
         <v>0.25</v>
       </c>
       <c r="D50" s="18"/>
@@ -1494,7 +1505,7 @@
       <c r="B51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="9">
         <v>1</v>
       </c>
       <c r="D51" s="18"/>
@@ -1507,7 +1518,7 @@
       <c r="B52" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="9">
         <v>1</v>
       </c>
       <c r="D52" s="18"/>
@@ -1520,7 +1531,7 @@
       <c r="B53" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="9">
         <v>0.75</v>
       </c>
       <c r="D53" s="18"/>
@@ -1533,7 +1544,7 @@
       <c r="B54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="9">
         <v>0.75</v>
       </c>
       <c r="D54" s="18"/>
@@ -1546,7 +1557,7 @@
       <c r="B55" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="9">
         <v>0.75</v>
       </c>
       <c r="D55" s="18"/>
@@ -1559,7 +1570,7 @@
       <c r="B56" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="9">
         <v>0.25</v>
       </c>
       <c r="D56" s="18"/>
@@ -1572,20 +1583,20 @@
       <c r="B57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="9">
         <v>0.75</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="21"/>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>43230</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="9">
         <v>1.25</v>
       </c>
       <c r="D58" s="18"/>
@@ -1598,7 +1609,7 @@
       <c r="B59" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="9">
         <v>0.75</v>
       </c>
       <c r="D59" s="18"/>
@@ -1611,7 +1622,7 @@
       <c r="B60" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C60" s="16">
+      <c r="C60" s="15">
         <v>0.5</v>
       </c>
       <c r="D60" s="18"/>
@@ -1624,7 +1635,7 @@
       <c r="B61" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="9">
         <v>1.5</v>
       </c>
       <c r="D61" s="18"/>
@@ -1637,7 +1648,7 @@
       <c r="B62" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="9">
         <v>0.5</v>
       </c>
       <c r="D62" s="18"/>
@@ -1650,7 +1661,7 @@
       <c r="B63" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="9">
         <v>0.5</v>
       </c>
       <c r="D63" s="18"/>
@@ -1663,7 +1674,7 @@
       <c r="B64" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="14">
         <v>1</v>
       </c>
       <c r="D64" s="18"/>
@@ -1676,7 +1687,7 @@
       <c r="B65" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="9">
         <v>1</v>
       </c>
       <c r="D65" s="18"/>
@@ -1689,7 +1700,7 @@
       <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="9">
         <v>1</v>
       </c>
       <c r="D66" s="19"/>
@@ -1702,15 +1713,15 @@
       <c r="B67" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="9">
         <v>0.75</v>
       </c>
       <c r="D67" s="20">
         <v>12</v>
       </c>
       <c r="E67" s="20">
-        <f>SUM(C67:C79)</f>
-        <v>16.75</v>
+        <f>SUM(C67:C82)</f>
+        <v>21.75</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,7 +1731,7 @@
       <c r="B68" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="9">
         <v>0.75</v>
       </c>
       <c r="D68" s="21"/>
@@ -1733,7 +1744,7 @@
       <c r="B69" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="9">
         <v>0.75</v>
       </c>
       <c r="D69" s="21"/>
@@ -1746,7 +1757,7 @@
       <c r="B70" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="9">
         <v>0.75</v>
       </c>
       <c r="D70" s="21"/>
@@ -1759,7 +1770,7 @@
       <c r="B71" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="9">
         <v>0.5</v>
       </c>
       <c r="D71" s="21"/>
@@ -1772,7 +1783,7 @@
       <c r="B72" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="10">
+      <c r="C72" s="9">
         <v>0.75</v>
       </c>
       <c r="D72" s="21"/>
@@ -1785,7 +1796,7 @@
       <c r="B73" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="9">
         <v>2.5</v>
       </c>
       <c r="D73" s="21"/>
@@ -1798,7 +1809,7 @@
       <c r="B74" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="9">
         <v>2.25</v>
       </c>
       <c r="D74" s="21"/>
@@ -1811,7 +1822,7 @@
       <c r="B75" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="9">
         <v>0.5</v>
       </c>
       <c r="D75" s="21"/>
@@ -1824,7 +1835,7 @@
       <c r="B76" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="9">
         <v>3</v>
       </c>
       <c r="D76" s="21"/>
@@ -1837,7 +1848,7 @@
       <c r="B77" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="9">
         <v>0.75</v>
       </c>
       <c r="D77" s="21"/>
@@ -1850,37 +1861,71 @@
       <c r="B78" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="9">
         <v>1.5</v>
       </c>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>43237</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="9">
         <v>2</v>
       </c>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="8"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
+      <c r="A80" s="3">
+        <v>43238</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" s="9">
+        <v>1</v>
+      </c>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>43238</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="16">
+        <v>43238</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="9">
-        <f>SUM(C5:C80)</f>
-        <v>103.5</v>
+      <c r="C83" s="8">
+        <f>SUM(C5:C82)</f>
+        <v>108.5</v>
       </c>
     </row>
   </sheetData>
@@ -1889,8 +1934,6 @@
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="E32:E34"/>
     <mergeCell ref="E35:E41"/>
-    <mergeCell ref="D67:D79"/>
-    <mergeCell ref="E67:E79"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="D24:D26"/>
     <mergeCell ref="D28:D31"/>
@@ -1898,6 +1941,8 @@
     <mergeCell ref="D35:D41"/>
     <mergeCell ref="D49:D66"/>
     <mergeCell ref="E49:E66"/>
+    <mergeCell ref="D67:D82"/>
+    <mergeCell ref="E67:E82"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D12"/>

</xml_diff>